<commit_message>
Excel, Screenshot and JSExecutor are learned
</commit_message>
<xml_diff>
--- a/src/test/java/day12_webtables_excel/ulkeler.xlsx
+++ b/src/test/java/day12_webtables_excel/ulkeler.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD72F3FB-F563-4469-A6C8-8EA3F4067799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2580A981-0288-4C26-B25E-03459BE71057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="576">
   <si>
     <t>Ülke (İngilizce)</t>
   </si>
@@ -1741,6 +1741,15 @@
   </si>
   <si>
     <t>Zimbabve</t>
+  </si>
+  <si>
+    <t>Nüfus</t>
+  </si>
+  <si>
+    <t>1500000</t>
+  </si>
+  <si>
+    <t>3000000</t>
   </si>
 </sst>
 </file>
@@ -2167,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:E191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1048576"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2178,7 +2187,7 @@
     <col min="1" max="4" width="25.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2191,8 +2200,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -2206,7 +2218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -2219,8 +2231,11 @@
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -2234,7 +2249,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -2248,7 +2263,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -2262,7 +2277,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -2275,8 +2290,11 @@
       <c r="D7" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -2290,7 +2308,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -2304,7 +2322,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -2318,7 +2336,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
@@ -2332,7 +2350,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -2346,7 +2364,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
@@ -2360,7 +2378,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -2374,7 +2392,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>46</v>
       </c>
@@ -2388,7 +2406,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>50</v>
       </c>

</xml_diff>